<commit_message>
Report_8_24 is going to be added to project :wink:
</commit_message>
<xml_diff>
--- a/Data (Don't be nosy !!!)/Data Gathering.xlsx
+++ b/Data (Don't be nosy !!!)/Data Gathering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQL-SP\Data (Don't be nosy !!!)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D4ACE4-8CF5-4719-92E6-BCFAB976BE24}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD7A054-5142-4040-A187-05E027EFCBA6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -203,14 +203,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -229,6 +229,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,7 +513,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:A14"/>
+      <selection activeCell="A10" sqref="A10:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,11 +542,11 @@
       <c r="C2" s="7"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -555,11 +556,11 @@
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -571,11 +572,11 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
@@ -631,21 +632,21 @@
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="7"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
+      <c r="A16" s="4"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="A17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="7"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
@@ -673,16 +674,17 @@
       <c r="C22" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A17:C17"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A10:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Report 8_24 ready to launch :triumph:
</commit_message>
<xml_diff>
--- a/Data (Don't be nosy !!!)/Data Gathering.xlsx
+++ b/Data (Don't be nosy !!!)/Data Gathering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQL-SP\Data (Don't be nosy !!!)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD7A054-5142-4040-A187-05E027EFCBA6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884FDA4F-9CC9-4C8A-8460-1B6DBAA1BADF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>شمال کرمان اجرای بند 5</t>
   </si>
@@ -85,13 +85,31 @@
   </si>
   <si>
     <t>2nd Week (1400/1/28)</t>
+  </si>
+  <si>
+    <t>ایلام ـ انجام بند 1 نامه ـ بخش دوم</t>
+  </si>
+  <si>
+    <t>frmMPFeederPeakDayNight.vb</t>
+  </si>
+  <si>
+    <t>Report_8_24.mrt</t>
+  </si>
+  <si>
+    <t>Report_8_24</t>
+  </si>
+  <si>
+    <t>Havades_App</t>
+  </si>
+  <si>
+    <t>frmMain.vb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,8 +124,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -138,8 +163,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -199,18 +230,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -230,6 +297,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A11"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,18 +620,18 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -556,11 +641,11 @@
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -572,11 +657,11 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
@@ -588,14 +673,14 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
@@ -604,58 +689,70 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
+      <c r="A14" s="9"/>
       <c r="B14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
+      <c r="A15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="6"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="A16" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="12"/>
+      <c r="C16" s="13"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
+      <c r="A17" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -673,17 +770,38 @@
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:A19"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A15:C15"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A15:C15"/>
     <mergeCell ref="A3:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adding Temp Folder :grin:
</commit_message>
<xml_diff>
--- a/Data (Don't be nosy !!!)/Data Gathering.xlsx
+++ b/Data (Don't be nosy !!!)/Data Gathering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQL-SP\Data (Don't be nosy !!!)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884FDA4F-9CC9-4C8A-8460-1B6DBAA1BADF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FFDBC08-9B82-41F1-818A-CAB18D2C784D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>شمال کرمان اجرای بند 5</t>
   </si>
@@ -103,6 +103,18 @@
   </si>
   <si>
     <t>frmMain.vb</t>
+  </si>
+  <si>
+    <t>آذربایجان غربی ـ تغییر در روش ایمپورت اطلاعات بارگیری و فایل اکسل مورد نظر</t>
+  </si>
+  <si>
+    <t>frmBaseTableNotstd</t>
+  </si>
+  <si>
+    <t>frmMPPostTransLoad</t>
+  </si>
+  <si>
+    <t>3rd Week (1400/2/4)</t>
   </si>
 </sst>
 </file>
@@ -278,6 +290,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -297,24 +327,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -597,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,18 +632,18 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="12"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -641,11 +653,11 @@
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -657,11 +669,11 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
@@ -673,14 +685,14 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
+      <c r="A10" s="15"/>
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
@@ -689,49 +701,49 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
+      <c r="A13" s="15"/>
       <c r="B13" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
+      <c r="A14" s="15"/>
       <c r="B14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="6"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="12"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="13"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -742,36 +754,44 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
+      <c r="A18" s="8"/>
       <c r="B18" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
+      <c r="A19" s="9"/>
       <c r="B19" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+      <c r="A20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="6"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
+      <c r="A21" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
+      <c r="A22" s="8"/>
+      <c r="B22" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
+      <c r="A23" s="9"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
     </row>
@@ -781,9 +801,11 @@
       <c r="C24" s="1"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
+      <c r="A25" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="11"/>
+      <c r="C25" s="12"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
@@ -791,7 +813,10 @@
       <c r="C26" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="14">
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A25:C25"/>
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="A2:C2"/>

</xml_diff>

<commit_message>
I ain't bitch like you :wink:
</commit_message>
<xml_diff>
--- a/Data (Don't be nosy !!!)/Data Gathering.xlsx
+++ b/Data (Don't be nosy !!!)/Data Gathering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQL-SP\Data (Don't be nosy !!!)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D24751B4-84EE-4620-A85B-25A1BDC563E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2506E3C4-EA7B-4CD0-A03E-7AD0431A5643}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>شمال کرمان اجرای بند 5</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>4th Week (1400/2/11)</t>
+  </si>
+  <si>
+    <t>Havades_App (Bargh_BaseTables)</t>
   </si>
 </sst>
 </file>
@@ -312,13 +315,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -328,6 +340,31 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -337,39 +374,14 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -651,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:C27"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,11 +688,11 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -729,14 +741,14 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
@@ -745,49 +757,49 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="6"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="13"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="15"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="16" t="s">
         <v>24</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -798,29 +810,29 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
+      <c r="A18" s="17"/>
       <c r="B18" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
+      <c r="A19" s="18"/>
       <c r="B19" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="13"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="15"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
-        <v>24</v>
+      <c r="A21" s="22" t="s">
+        <v>35</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>27</v>
@@ -830,68 +842,66 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
+      <c r="A22" s="23"/>
       <c r="B22" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="23"/>
+      <c r="B23" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="24"/>
+      <c r="B24" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="6"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="20"/>
-      <c r="C25" s="21"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="9"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="6"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="9"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="18"/>
+      <c r="A29" s="11"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
     </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="12"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A24:C24"/>
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="A2:C2"/>
@@ -903,6 +913,13 @@
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A25:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Omid's Back On Track :wink:
</commit_message>
<xml_diff>
--- a/Data (Don't be nosy !!!)/Data Gathering.xlsx
+++ b/Data (Don't be nosy !!!)/Data Gathering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQL-SP\Data (Don't be nosy !!!)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2506E3C4-EA7B-4CD0-A03E-7AD0431A5643}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C86395-E59A-4BEE-B3CF-18025991A456}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
     <t>شمال کرمان اجرای بند 5</t>
   </si>
@@ -133,13 +133,37 @@
   </si>
   <si>
     <t>Havades_App (Bargh_BaseTables)</t>
+  </si>
+  <si>
+    <t>TZServicesCSharp</t>
+  </si>
+  <si>
+    <t>غرب مازندران ـ ایجاد وب سرویس متناظر گزارش 14-1 در نرم افزار</t>
+  </si>
+  <si>
+    <t>&lt;Host-Name&gt;/Reports/gmaz_report_sabz</t>
+  </si>
+  <si>
+    <t>RestReports.aspx.cs</t>
+  </si>
+  <si>
+    <t>HavadesReports.asmx.cs</t>
+  </si>
+  <si>
+    <t>Report_14_1</t>
+  </si>
+  <si>
+    <t>spGMaz_Report_14_1</t>
+  </si>
+  <si>
+    <t>???</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,8 +193,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -213,8 +250,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -311,17 +354,71 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -331,57 +428,23 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -663,10 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,9 +737,10 @@
     <col min="1" max="1" width="27.42578125" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
     <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="5" max="7" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -686,36 +750,65 @@
       <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="9"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="B2" s="16"/>
+      <c r="C2" s="17"/>
+      <c r="E2" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="16"/>
+      <c r="G2" s="17"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="E3" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="22"/>
+      <c r="G3" s="23"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="E4" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="16"/>
+      <c r="G4" s="17"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="E5" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
@@ -723,15 +816,29 @@
       <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="E6" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="26"/>
+      <c r="G6" s="28"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="E7" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="29" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="1" t="s">
         <v>8</v>
@@ -739,67 +846,85 @@
       <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="E8" s="25"/>
+      <c r="F8" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="19"/>
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
+      <c r="E10" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="19"/>
       <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+      <c r="E11" s="25"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="19"/>
       <c r="B13" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="19"/>
       <c r="B14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="9"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+      <c r="B15" s="16"/>
+      <c r="C15" s="17"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="15"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="11"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="12" t="s">
         <v>24</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -810,28 +935,28 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
+      <c r="A19" s="14"/>
       <c r="B19" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="15"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="8" t="s">
         <v>35</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -842,66 +967,68 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="23"/>
+      <c r="A22" s="8"/>
       <c r="B22" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="23"/>
+      <c r="A23" s="8"/>
       <c r="B23" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C23" s="1"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="24"/>
+      <c r="A24" s="8"/>
       <c r="B24" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C24" s="1"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="8"/>
-      <c r="C25" s="9"/>
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" s="5"/>
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
       <c r="C26" s="6"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="9"/>
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
+      <c r="A29" s="5"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
+      <c r="A30" s="5"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="21">
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:A24"/>
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="A2:C2"/>
@@ -913,13 +1040,6 @@
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="A25:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Not in the mood to explain :weary:
</commit_message>
<xml_diff>
--- a/Data (Don't be nosy !!!)/Data Gathering.xlsx
+++ b/Data (Don't be nosy !!!)/Data Gathering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQL-SP\Data (Don't be nosy !!!)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C86395-E59A-4BEE-B3CF-18025991A456}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6E8461-D046-4CC6-87AC-2B27FA1B9133}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -379,71 +379,71 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -729,7 +729,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10:G11"/>
+      <selection activeCell="E6" sqref="E6:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,28 +761,28 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="17"/>
-      <c r="E2" s="15" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="18"/>
+      <c r="E2" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="18"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="E3" s="21" t="s">
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="E3" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="22"/>
-      <c r="G3" s="23"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="21"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -790,23 +790,23 @@
         <v>1</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="16"/>
-      <c r="G4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="18"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="E5" s="20" t="s">
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="E5" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -816,25 +816,25 @@
       <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="26"/>
-      <c r="G6" s="28"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="12"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="E7" s="24" t="s">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="E7" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="27" t="s">
+      <c r="F7" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="29" t="s">
+      <c r="G7" s="8" t="s">
         <v>41</v>
       </c>
     </row>
@@ -846,85 +846,85 @@
       <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="25"/>
-      <c r="F8" s="27" t="s">
+      <c r="E8" s="14"/>
+      <c r="F8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="30" t="s">
+      <c r="G8" s="9" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="13" t="s">
         <v>43</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
+      <c r="A11" s="31"/>
       <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="E11" s="25"/>
+      <c r="E11" s="14"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
+      <c r="A13" s="31"/>
       <c r="B13" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
+      <c r="A14" s="31"/>
       <c r="B14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="18"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="11"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="26"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="27" t="s">
         <v>24</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -935,28 +935,28 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
+      <c r="A18" s="28"/>
       <c r="B18" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
+      <c r="A19" s="29"/>
       <c r="B19" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="23" t="s">
         <v>35</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -967,21 +967,21 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
+      <c r="A22" s="23"/>
       <c r="B22" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
+      <c r="A23" s="23"/>
       <c r="B23" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C23" s="1"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
+      <c r="A24" s="23"/>
       <c r="B24" s="1" t="s">
         <v>32</v>
       </c>
@@ -1019,14 +1019,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="A21:A24"/>
     <mergeCell ref="A16:C16"/>
@@ -1040,6 +1032,14 @@
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A3:C3"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Omid is back :triumph:
</commit_message>
<xml_diff>
--- a/Data (Don't be nosy !!!)/Data Gathering.xlsx
+++ b/Data (Don't be nosy !!!)/Data Gathering.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQL-SP\Data (Don't be nosy !!!)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6E8461-D046-4CC6-87AC-2B27FA1B9133}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952902DC-06C1-4040-9C16-D634DF75DEE4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>شمال کرمان اجرای بند 5</t>
   </si>
@@ -156,7 +156,13 @@
     <t>spGMaz_Report_14_1</t>
   </si>
   <si>
-    <t>???</t>
+    <t>البرز ـ اجرای بند 1-2 نامه مطابق توضیحات</t>
+  </si>
+  <si>
+    <t>frmMonitorErja.vb</t>
+  </si>
+  <si>
+    <t>ViewMonitoringErja</t>
   </si>
 </sst>
 </file>
@@ -369,7 +375,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -382,6 +388,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -397,16 +443,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -416,35 +452,13 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -729,7 +743,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:G6"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,28 +775,28 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="18"/>
-      <c r="E2" s="16" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="20"/>
+      <c r="E2" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="17"/>
-      <c r="G2" s="18"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="20"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="E3" s="19" t="s">
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="E3" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="20"/>
-      <c r="G3" s="21"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="31"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -790,23 +804,23 @@
         <v>1</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="20"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="E5" s="15" t="s">
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="E5" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -816,19 +830,19 @@
       <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="12"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="26"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="E7" s="13" t="s">
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="E7" s="27" t="s">
         <v>36</v>
       </c>
       <c r="F7" s="7" t="s">
@@ -846,7 +860,7 @@
       <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="14"/>
+      <c r="E8" s="28"/>
       <c r="F8" s="7" t="s">
         <v>40</v>
       </c>
@@ -855,76 +869,82 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="E9" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="E10" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
+      <c r="A14" s="22"/>
       <c r="B14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="18"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="20"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="26"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="14"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="15" t="s">
         <v>24</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -935,28 +955,28 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="28"/>
+      <c r="A18" s="16"/>
       <c r="B18" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="29"/>
+      <c r="A19" s="17"/>
       <c r="B19" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="11" t="s">
         <v>35</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -967,21 +987,21 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="23"/>
+      <c r="A22" s="11"/>
       <c r="B22" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="23"/>
+      <c r="A23" s="11"/>
       <c r="B23" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C23" s="1"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="23"/>
+      <c r="A24" s="11"/>
       <c r="B24" s="1" t="s">
         <v>32</v>
       </c>
@@ -1018,7 +1038,14 @@
       <c r="C30" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="20">
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="A21:A24"/>
     <mergeCell ref="A16:C16"/>
@@ -1032,14 +1059,6 @@
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A3:C3"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ahvaz Report Finished :triumph:
</commit_message>
<xml_diff>
--- a/Data (Don't be nosy !!!)/Data Gathering.xlsx
+++ b/Data (Don't be nosy !!!)/Data Gathering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQL-SP\Data (Don't be nosy !!!)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952902DC-06C1-4040-9C16-D634DF75DEE4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87AE706A-4D5A-46DE-B115-761F35B187E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
   <si>
     <t>شمال کرمان اجرای بند 5</t>
   </si>
@@ -163,6 +163,15 @@
   </si>
   <si>
     <t>ViewMonitoringErja</t>
+  </si>
+  <si>
+    <t>rptEzamEkipInfo.rpt</t>
+  </si>
+  <si>
+    <t>rptEzamEkipInfo_Mode2.rpt</t>
+  </si>
+  <si>
+    <t>اهواز ـ اضافه نمودن تعداد قطعات مصرفی نو و مستعمل ، با و بدون حواله انبار، به گزارش دستور کار انجام شده.</t>
   </si>
 </sst>
 </file>
@@ -388,6 +397,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -412,54 +459,14 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -743,7 +750,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,16 +782,16 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="20"/>
-      <c r="E2" s="18" t="s">
+      <c r="B2" s="18"/>
+      <c r="C2" s="19"/>
+      <c r="E2" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="19"/>
-      <c r="G2" s="20"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="19"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
@@ -792,11 +799,11 @@
       </c>
       <c r="B3" s="23"/>
       <c r="C3" s="23"/>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="30"/>
-      <c r="G3" s="31"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="22"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -804,11 +811,11 @@
         <v>1</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="19"/>
-      <c r="G4" s="20"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="19"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
@@ -830,11 +837,11 @@
       <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="25"/>
-      <c r="G6" s="26"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="13"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
@@ -842,7 +849,7 @@
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="23"/>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="14" t="s">
         <v>36</v>
       </c>
       <c r="F7" s="7" t="s">
@@ -860,7 +867,7 @@
       <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="28"/>
+      <c r="E8" s="15"/>
       <c r="F8" s="7" t="s">
         <v>40</v>
       </c>
@@ -869,29 +876,29 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="E9" s="34" t="s">
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="E9" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
+      <c r="A10" s="33"/>
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="35" t="s">
+      <c r="E10" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="34" t="s">
         <v>44</v>
       </c>
       <c r="G10" s="1" t="s">
@@ -899,52 +906,66 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
+      <c r="A11" s="33"/>
       <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
+      <c r="E11" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="E12" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
+      <c r="A13" s="33"/>
       <c r="B13" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="1"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="9"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
+      <c r="A14" s="33"/>
       <c r="B14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="20"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="19"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="14"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="28"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="29" t="s">
         <v>24</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -955,28 +976,28 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
+      <c r="A18" s="30"/>
       <c r="B18" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
+      <c r="A19" s="31"/>
       <c r="B19" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="25" t="s">
         <v>35</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -987,21 +1008,21 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
+      <c r="A22" s="25"/>
       <c r="B22" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
+      <c r="A23" s="25"/>
       <c r="B23" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C23" s="1"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
+      <c r="A24" s="25"/>
       <c r="B24" s="1" t="s">
         <v>32</v>
       </c>
@@ -1038,14 +1059,9 @@
       <c r="C30" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
+  <mergeCells count="22">
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E12:E13"/>
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="A21:A24"/>
     <mergeCell ref="A16:C16"/>
@@ -1059,6 +1075,13 @@
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A3:C3"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>